<commit_message>
updated monte carlo/sensitivity contact length
</commit_message>
<xml_diff>
--- a/research/Monte_carlo/inputs/NBNL_plume_SA.xlsx
+++ b/research/Monte_carlo/inputs/NBNL_plume_SA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://kwrwater-my.sharepoint.com/personal/alex_hockin_kwrwater_nl/Documents/VEWIN Permatie/pipepermcalc/research/Monte_carlo/inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="133" documentId="8_{EBD4BD38-97D2-4A1B-AC9C-0CB3E2990D6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6C21106B-4A49-484C-91AD-E685D6559AB1}"/>
+  <xr:revisionPtr revIDLastSave="137" documentId="8_{EBD4BD38-97D2-4A1B-AC9C-0CB3E2990D6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{873D726F-F1EA-41C6-956A-4B681377B988}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17790" xr2:uid="{264446DA-FF6B-4067-B3E4-C2382FFFE8DA}"/>
+    <workbookView xWindow="-28920" yWindow="15855" windowWidth="29040" windowHeight="15990" xr2:uid="{264446DA-FF6B-4067-B3E4-C2382FFFE8DA}"/>
   </bookViews>
   <sheets>
     <sheet name="plume_SA" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="39">
   <si>
     <t>Location</t>
   </si>
@@ -146,10 +146,13 @@
     <t>Stantec</t>
   </si>
   <si>
-    <t>Old contact lengths</t>
-  </si>
-  <si>
-    <t>New contact lengths</t>
+    <t>Old plume lengths</t>
+  </si>
+  <si>
+    <t>New plume lengths</t>
+  </si>
+  <si>
+    <t>Final data</t>
   </si>
 </sst>
 </file>
@@ -614,25 +617,28 @@
   <dimension ref="B2:W36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="W31" sqref="W31"/>
+      <selection activeCell="S3" sqref="S3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="29.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="3" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="S2" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B3" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>15</v>
       </c>
@@ -652,7 +658,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>16</v>
       </c>
@@ -674,7 +680,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
         <v>17</v>
       </c>
@@ -693,7 +699,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B7" s="2">
         <v>43564</v>
       </c>
@@ -712,7 +718,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:23" x14ac:dyDescent="0.35">
       <c r="S8" t="s">
         <v>4</v>
       </c>
@@ -728,7 +734,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
         <v>0</v>
       </c>
@@ -756,7 +762,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
         <v>1</v>
       </c>
@@ -789,7 +795,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
         <v>2</v>
       </c>
@@ -819,7 +825,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B12" t="s">
         <v>3</v>
       </c>
@@ -845,7 +851,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B13" t="s">
         <v>4</v>
       </c>
@@ -871,7 +877,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="14" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B14" t="s">
         <v>5</v>
       </c>
@@ -897,7 +903,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="15" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B15" t="s">
         <v>6</v>
       </c>
@@ -926,7 +932,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B16" t="s">
         <v>7</v>
       </c>
@@ -955,7 +961,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="21" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:22" x14ac:dyDescent="0.35">
       <c r="U21" t="s">
         <v>36</v>
       </c>
@@ -963,7 +969,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="22" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:22" x14ac:dyDescent="0.35">
       <c r="U22">
         <v>0.5</v>
       </c>
@@ -971,7 +977,7 @@
         <v>1.9544100476116797</v>
       </c>
     </row>
-    <row r="23" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:22" x14ac:dyDescent="0.35">
       <c r="U23">
         <v>0.5</v>
       </c>
@@ -979,7 +985,7 @@
         <v>2.4462677409178384</v>
       </c>
     </row>
-    <row r="24" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:22" x14ac:dyDescent="0.35">
       <c r="B24" t="s">
         <v>18</v>
       </c>
@@ -990,7 +996,7 @@
         <v>2.763953195770684</v>
       </c>
     </row>
-    <row r="25" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:22" x14ac:dyDescent="0.35">
       <c r="B25" s="3" t="s">
         <v>19</v>
       </c>
@@ -1001,7 +1007,7 @@
         <v>2.8322092316478891</v>
       </c>
     </row>
-    <row r="26" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:22" x14ac:dyDescent="0.35">
       <c r="B26" t="s">
         <v>20</v>
       </c>
@@ -1012,7 +1018,7 @@
         <v>3.0066594033278284</v>
       </c>
     </row>
-    <row r="27" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:22" x14ac:dyDescent="0.35">
       <c r="B27" t="s">
         <v>21</v>
       </c>
@@ -1023,7 +1029,7 @@
         <v>3.4595450164017998</v>
       </c>
     </row>
-    <row r="28" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:22" x14ac:dyDescent="0.35">
       <c r="B28" s="2">
         <v>43594</v>
       </c>
@@ -1034,7 +1040,7 @@
         <v>3.477898169151024</v>
       </c>
     </row>
-    <row r="29" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:22" x14ac:dyDescent="0.35">
       <c r="F29" t="s">
         <v>29</v>
       </c>
@@ -1045,7 +1051,7 @@
         <v>3.6563663957157262</v>
       </c>
     </row>
-    <row r="30" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:22" x14ac:dyDescent="0.35">
       <c r="B30" t="s">
         <v>0</v>
       </c>
@@ -1074,7 +1080,7 @@
         <v>4.5135166683820502</v>
       </c>
     </row>
-    <row r="31" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:22" x14ac:dyDescent="0.35">
       <c r="B31" t="s">
         <v>22</v>
       </c>
@@ -1102,7 +1108,7 @@
         <v>5.2320789569544912</v>
       </c>
     </row>
-    <row r="32" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:22" x14ac:dyDescent="0.35">
       <c r="B32" t="s">
         <v>23</v>
       </c>
@@ -1130,7 +1136,7 @@
         <v>7.9788456080286538</v>
       </c>
     </row>
-    <row r="33" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:22" x14ac:dyDescent="0.35">
       <c r="B33" t="s">
         <v>24</v>
       </c>
@@ -1158,7 +1164,7 @@
         <v>16.390654164465779</v>
       </c>
     </row>
-    <row r="34" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:22" x14ac:dyDescent="0.35">
       <c r="B34" t="s">
         <v>25</v>
       </c>
@@ -1180,7 +1186,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:22" x14ac:dyDescent="0.35">
       <c r="B35" t="s">
         <v>26</v>
       </c>
@@ -1202,7 +1208,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="36" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:22" x14ac:dyDescent="0.35">
       <c r="H36" t="s">
         <v>32</v>
       </c>

</xml_diff>

<commit_message>
updates to monte carlo simulations, plotting
</commit_message>
<xml_diff>
--- a/research/Monte_carlo/inputs/NBNL_plume_SA.xlsx
+++ b/research/Monte_carlo/inputs/NBNL_plume_SA.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="137" documentId="8_{EBD4BD38-97D2-4A1B-AC9C-0CB3E2990D6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{873D726F-F1EA-41C6-956A-4B681377B988}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="15855" windowWidth="29040" windowHeight="15990" xr2:uid="{264446DA-FF6B-4067-B3E4-C2382FFFE8DA}"/>
+    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="17550" xr2:uid="{264446DA-FF6B-4067-B3E4-C2382FFFE8DA}"/>
   </bookViews>
   <sheets>
     <sheet name="plume_SA" sheetId="1" r:id="rId1"/>
@@ -315,6 +315,10 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -616,16 +620,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4AE1DBA-7883-4910-9B40-0442EC117BCC}">
   <dimension ref="B2:W36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S3" sqref="S3"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="S4" sqref="S4:W16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="29.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:23" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>18</v>
       </c>
@@ -633,12 +637,12 @@
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="2:23" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="2:23" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>15</v>
       </c>
@@ -658,7 +662,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="2:23" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>16</v>
       </c>
@@ -680,7 +684,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="2:23" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>17</v>
       </c>
@@ -699,7 +703,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="2:23" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B7" s="2">
         <v>43564</v>
       </c>
@@ -718,7 +722,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="2:23" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:23" x14ac:dyDescent="0.25">
       <c r="S8" t="s">
         <v>4</v>
       </c>
@@ -734,7 +738,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="2:23" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>0</v>
       </c>
@@ -762,7 +766,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="2:23" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>1</v>
       </c>
@@ -795,7 +799,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="2:23" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>2</v>
       </c>
@@ -825,7 +829,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="2:23" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>3</v>
       </c>
@@ -851,7 +855,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="2:23" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>4</v>
       </c>
@@ -877,7 +881,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="14" spans="2:23" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>5</v>
       </c>
@@ -903,7 +907,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="15" spans="2:23" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>6</v>
       </c>
@@ -932,7 +936,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="2:23" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>7</v>
       </c>
@@ -961,7 +965,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="21" spans="2:22" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:22" x14ac:dyDescent="0.25">
       <c r="U21" t="s">
         <v>36</v>
       </c>
@@ -969,7 +973,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="22" spans="2:22" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:22" x14ac:dyDescent="0.25">
       <c r="U22">
         <v>0.5</v>
       </c>
@@ -977,7 +981,7 @@
         <v>1.9544100476116797</v>
       </c>
     </row>
-    <row r="23" spans="2:22" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:22" x14ac:dyDescent="0.25">
       <c r="U23">
         <v>0.5</v>
       </c>
@@ -985,7 +989,7 @@
         <v>2.4462677409178384</v>
       </c>
     </row>
-    <row r="24" spans="2:22" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>18</v>
       </c>
@@ -996,7 +1000,7 @@
         <v>2.763953195770684</v>
       </c>
     </row>
-    <row r="25" spans="2:22" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B25" s="3" t="s">
         <v>19</v>
       </c>
@@ -1007,7 +1011,7 @@
         <v>2.8322092316478891</v>
       </c>
     </row>
-    <row r="26" spans="2:22" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>20</v>
       </c>
@@ -1018,7 +1022,7 @@
         <v>3.0066594033278284</v>
       </c>
     </row>
-    <row r="27" spans="2:22" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>21</v>
       </c>
@@ -1029,7 +1033,7 @@
         <v>3.4595450164017998</v>
       </c>
     </row>
-    <row r="28" spans="2:22" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B28" s="2">
         <v>43594</v>
       </c>
@@ -1040,7 +1044,7 @@
         <v>3.477898169151024</v>
       </c>
     </row>
-    <row r="29" spans="2:22" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:22" x14ac:dyDescent="0.25">
       <c r="F29" t="s">
         <v>29</v>
       </c>
@@ -1051,7 +1055,7 @@
         <v>3.6563663957157262</v>
       </c>
     </row>
-    <row r="30" spans="2:22" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>0</v>
       </c>
@@ -1080,7 +1084,7 @@
         <v>4.5135166683820502</v>
       </c>
     </row>
-    <row r="31" spans="2:22" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>22</v>
       </c>
@@ -1108,7 +1112,7 @@
         <v>5.2320789569544912</v>
       </c>
     </row>
-    <row r="32" spans="2:22" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>23</v>
       </c>
@@ -1136,7 +1140,7 @@
         <v>7.9788456080286538</v>
       </c>
     </row>
-    <row r="33" spans="2:22" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>24</v>
       </c>
@@ -1164,7 +1168,7 @@
         <v>16.390654164465779</v>
       </c>
     </row>
-    <row r="34" spans="2:22" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>25</v>
       </c>
@@ -1186,7 +1190,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="2:22" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>26</v>
       </c>
@@ -1208,7 +1212,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="36" spans="2:22" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:22" x14ac:dyDescent="0.25">
       <c r="H36" t="s">
         <v>32</v>
       </c>

</xml_diff>